<commit_message>
Add more vol test data.  Linked Group test data to Volunteer test data (IDs and such).
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/Volunteer.xlsx
+++ b/UT.Vol.BLL/HelperFiles/Volunteer.xlsx
@@ -5,12 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="917" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -40,7 +38,7 @@
     <t>Query</t>
   </si>
   <si>
-    <t>[Vol].[tblVolunteer]</t>
+    <t>[VolTeer].[Vol].[tblVolunteer]</t>
   </si>
   <si>
     <t>ffece320-d093-4ba7-a56c-6d7dc8127a4c</t>
@@ -198,6 +196,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,10 +267,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -328,7 +327,7 @@
       </c>
       <c r="G2" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A2&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "' ,'" &amp; E2 &amp; "','" &amp; F2 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'ffece320-d093-4ba7-a56c-6d7dc8127a4c','Jacqualine','Yajaira' ,'Spruill','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'ffece320-d093-4ba7-a56c-6d7dc8127a4c','Jacqualine','Yajaira' ,'Spruill','1')</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,7 +351,7 @@
       </c>
       <c r="G3" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A3&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B3 &amp; "','" &amp; C3 &amp; "','" &amp; D3 &amp; "' ,'" &amp; E3 &amp; "','" &amp; F3 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'eafcce35-6200-4c5a-aae1-6fad06f3467a','Gussie','Curtis' ,'Mckinny','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'eafcce35-6200-4c5a-aae1-6fad06f3467a','Gussie','Curtis' ,'Mckinny','1')</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,7 +375,7 @@
       </c>
       <c r="G4" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A4&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B4 &amp; "','" &amp; C4 &amp; "','" &amp; D4 &amp; "' ,'" &amp; E4 &amp; "','" &amp; F4 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'df91056c-6383-4fb6-b006-c6cee3df959b','Julia','Willena' ,'Corella','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'df91056c-6383-4fb6-b006-c6cee3df959b','Julia','Willena' ,'Corella','1')</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,7 +399,7 @@
       </c>
       <c r="G5" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A5&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "' ,'" &amp; E5 &amp; "','" &amp; F5 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8b6d44cd-6fca-4d42-afbe-a91fa43c4f4b','Dakota','Joanie' ,'Greb','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8b6d44cd-6fca-4d42-afbe-a91fa43c4f4b','Dakota','Joanie' ,'Greb','1')</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +423,7 @@
       </c>
       <c r="G6" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A6&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "' ,'" &amp; E6 &amp; "','" &amp; F6 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '9b588220-7bd4-415e-ae65-760b40929fdc','Mercedez','Lissette' ,'Auxier','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '9b588220-7bd4-415e-ae65-760b40929fdc','Mercedez','Lissette' ,'Auxier','1')</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,7 +447,7 @@
       </c>
       <c r="G7" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A7&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B7 &amp; "','" &amp; C7 &amp; "','" &amp; D7 &amp; "' ,'" &amp; E7 &amp; "','" &amp; F7 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8a2e0c86-fd6e-4db0-9e24-b32506a66b3b','Samual','Cristi' ,'Moone','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8a2e0c86-fd6e-4db0-9e24-b32506a66b3b','Samual','Cristi' ,'Moone','1')</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,7 +471,7 @@
       </c>
       <c r="G8" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A8&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B8 &amp; "','" &amp; C8 &amp; "','" &amp; D8 &amp; "' ,'" &amp; E8 &amp; "','" &amp; F8 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8ba077f8-4e8b-45af-99f3-cb099de2dfcc','Shannon','Angelic' ,'Leventhal','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '8ba077f8-4e8b-45af-99f3-cb099de2dfcc','Shannon','Angelic' ,'Leventhal','1')</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +495,7 @@
       </c>
       <c r="G9" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A9&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B9 &amp; "','" &amp; C9 &amp; "','" &amp; D9 &amp; "' ,'" &amp; E9 &amp; "','" &amp; F9 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '72f51403-53b0-4a74-ab2b-d7fdd9d5657c','Porsha','Trula' ,'Streeter','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '72f51403-53b0-4a74-ab2b-d7fdd9d5657c','Porsha','Trula' ,'Streeter','1')</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +519,7 @@
       </c>
       <c r="G10" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A10&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B10 &amp; "','" &amp; C10 &amp; "','" &amp; D10 &amp; "' ,'" &amp; E10 &amp; "','" &amp; F10 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'ca8a0ae5-1a4a-49fe-af42-015b6a17274b','Racquel','Lovetta' ,'Tuma','1')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( 'ca8a0ae5-1a4a-49fe-af42-015b6a17274b','Racquel','Lovetta' ,'Tuma','1')</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,10 +543,11 @@
       </c>
       <c r="G11" s="1" t="str">
         <f aca="false">"INSERT INTO "&amp;A11&amp;" ([" &amp;B$1 &amp;"],["&amp;C$1&amp;"],["&amp;D$1&amp;"],["&amp;E$1&amp;"],["&amp;F$1&amp;"]) VALUES ( '" &amp; B11 &amp; "','" &amp; C11 &amp; "','" &amp; D11 &amp; "' ,'" &amp; E11 &amp; "','" &amp; F11 &amp; "')"</f>
-        <v>INSERT INTO [Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '24a4e8af-c01e-4297-a1bb-f8356b259484','Luanna','Tangela' ,'Ruddell','0')</v>
+        <v>INSERT INTO [VolTeer].[Vol].[tblVolunteer] ([VolID],[VolFirstName],[VolMiddleName],[VolLastName],[ActiveFlg]) VALUES ( '24a4e8af-c01e-4297-a1bb-f8356b259484','Luanna','Tangela' ,'Ruddell','0')</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -557,56 +557,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>